<commit_message>
comments to metadata examples
</commit_message>
<xml_diff>
--- a/metadata-examples.xlsx
+++ b/metadata-examples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sotsiaalministeerium.ee\dfs\Kasutajad\rutt.lindstrom\Documents\Terminoloogia-Haldus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igor/source/tis/terminology-migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A993E9D0-9E68-4877-802D-4E0B21295336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF54BBD-787A-E940-8C63-B80309B2664F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29775" yWindow="3795" windowWidth="26595" windowHeight="9525" xr2:uid="{2916EE3D-FE7D-4C58-9D3A-4F5149FE7FE9}"/>
+    <workbookView xWindow="320" yWindow="5760" windowWidth="25600" windowHeight="9520" xr2:uid="{2916EE3D-FE7D-4C58-9D3A-4F5149FE7FE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,60 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+    <author>tc={07464E29-D51C-CD4F-A11E-3FEE8A2A43CC}</author>
+  </authors>
+  <commentList>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{BB220C53-56E6-AD48-B7DB-C1BFA2321BB6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Removed "_"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="1" shapeId="0" xr:uid="{07464E29-D51C-CD4F-A11E-3FEE8A2A43CC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Removed “_”</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
   <si>
     <t>FHIR ressurss</t>
   </si>
@@ -217,13 +269,94 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>https://fhir.ee/CodeSystem/AK</t>
+  </si>
+  <si>
+    <t>https://pub.e-tervis.ee/classifications/Abivahendid%20ja%20meditsiiniseadmed/4</t>
+  </si>
+  <si>
+    <t>Pubkeskuse URL</t>
+  </si>
+  <si>
+    <t>Kommentaar</t>
+  </si>
+  <si>
+    <t>Seda ei ole vaja tekkitada?</t>
+  </si>
+  <si>
+    <t>Tulemus</t>
+  </si>
+  <si>
+    <t>https://termx.kodality.dev/api/fhir/ValueSet/ebmeds-diagnooside-filter@2/$expand?includeDesignations=true&amp;displayLanguage=et</t>
+  </si>
+  <si>
+    <t>https://termx.kodality.dev/api/fhir/ValueSet/abivahendid-meditsiiniseadmed@4/$expand?includeDesignations=true</t>
+  </si>
+  <si>
+    <t>https://termx.kodality.dev/api/fhir/CodeSystem/abivahendid-meditsiiniseadmed@4</t>
+  </si>
+  <si>
+    <t>Kas antud juhul supplement nime sees vajalik?</t>
+  </si>
+  <si>
+    <t>https://github.com/TEHIK-EE/terminology-migration/issues/18</t>
+  </si>
+  <si>
+    <t>Nimi on AK: https://klassifikaatorid.stat.ee/item/stat.ee/371ce1b7-030a-450e-985a-0bd232d76d73/3</t>
+  </si>
+  <si>
+    <t>https://termx.kodality.dev/resources/code-systems/AK/versions/2008/summary</t>
+  </si>
+  <si>
+    <t>OID-id tulevad loedi kälge</t>
+  </si>
+  <si>
+    <t>Ei paneks sidekriipse vahele</t>
+  </si>
+  <si>
+    <t>https://pub.e-tervis.ee/classifications/ER_Müügiloata%20taotluse%20põhjendus/1</t>
+  </si>
+  <si>
+    <t>https://termx.kodality.dev/api/fhir/CodeSystem/er-myygiloata-taotluse-pohjendus@1.0.0</t>
+  </si>
+  <si>
+    <t>https://termx.kodality.dev/api/fhir/ValueSet/er-myygiloata-taotluse-pohjendus@1/$expand?includeDesignations=true</t>
+  </si>
+  <si>
+    <t>https://termx.kodality.dev/api/fhir/CodeSystem/ema-oletatav-nakatumisviis@1.0.0</t>
+  </si>
+  <si>
+    <t>https://termx.kodality.dev/api/fhir/ValueSet/ema-oletatav-nakatumisviis@1/$expand?includeDesignations=true&amp;displayLanguage=et</t>
+  </si>
+  <si>
+    <t>https://pub.e-tervis.ee/classifications/MTK_Elektrokardiostimulatsiooni%20režiim/1</t>
+  </si>
+  <si>
+    <t>https://pub.e-tervis.ee/classifications/Emalt%20nakkuse%20saanu%20ema%20oletatav%20nakatumise%20viis/1</t>
+  </si>
+  <si>
+    <t>https://termx.kodality.dev/api/fhir/CodeSystem/mtk-elektrokardiostimulatsiooni-rezhiim@1.0.0</t>
+  </si>
+  <si>
+    <t>https://termx.kodality.dev/api/fhir/ValueSet/mtk-elektrokardiostimulatsiooni-rezhiim@1/$expand?includeDesignations=true&amp;displayLanguage=et</t>
+  </si>
+  <si>
+    <t>https://pub.e-tervis.ee/classifications/Farmakogeneetilise%20uuringu%20(geeniprodukti%20funktsioon)%20vastus/2</t>
+  </si>
+  <si>
+    <t>SNOMED, only VS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,6 +447,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -336,20 +499,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -366,6 +531,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Igor Bossenko" id="{90391009-2C50-404E-9C44-AA500A014AA6}" userId="S::igboss@ttu.ee::0681fb89-f5ce-47ec-9f60-588dd162ca24" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -663,64 +834,72 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F6" dT="2023-08-24T11:47:55.38" personId="{90391009-2C50-404E-9C44-AA500A014AA6}" id="{07464E29-D51C-CD4F-A11E-3FEE8A2A43CC}">
+    <text>Removed “_”</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6059A022-ED99-42E5-B5F1-45B40130E12C}">
-  <dimension ref="A1:K24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6059A022-ED99-42E5-B5F1-45B40130E12C}">
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="24.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.81640625" customWidth="1"/>
-    <col min="2" max="2" width="3.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="27.1796875" customWidth="1"/>
-    <col min="7" max="7" width="4.6328125" customWidth="1"/>
-    <col min="8" max="8" width="34.6328125" customWidth="1"/>
-    <col min="9" max="9" width="4.81640625" customWidth="1"/>
-    <col min="10" max="10" width="50.6328125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="18.90625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.81640625" customWidth="1"/>
-    <col min="13" max="13" width="16.08984375" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="4"/>
+    <col min="11" max="11" width="24.6640625" style="1"/>
+    <col min="13" max="13" width="48.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="L1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -753,8 +932,14 @@
       <c r="K2" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="L2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -771,24 +956,30 @@
         <v>31</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" ref="G3:G13" si="0">LEN(F3)</f>
+        <f t="shared" ref="G3:G12" si="0">LEN(F3)</f>
         <v>28</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>37</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I13" si="1">LEN(H3)</f>
+        <f t="shared" ref="I3:I12" si="1">LEN(H3)</f>
         <v>40</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>36</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="M3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -821,8 +1012,11 @@
       <c r="K4" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="N4" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -855,8 +1049,14 @@
       <c r="K5" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="M5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -866,17 +1066,17 @@
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>24</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>25</v>
       </c>
       <c r="I6" s="4">
@@ -889,8 +1089,11 @@
       <c r="K6" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="N6" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -903,14 +1106,14 @@
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>25</v>
       </c>
       <c r="I7" s="4">
@@ -923,8 +1126,14 @@
       <c r="K7" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="L7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -957,8 +1166,11 @@
       <c r="K8" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="N8" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
@@ -991,8 +1203,14 @@
       <c r="K9" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="L9" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
@@ -1005,14 +1223,14 @@
       <c r="D10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>45</v>
       </c>
       <c r="I10" s="4">
@@ -1025,8 +1243,11 @@
       <c r="K10" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="N10" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -1039,14 +1260,14 @@
       <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>45</v>
       </c>
       <c r="I11" s="4">
@@ -1059,9 +1280,15 @@
       <c r="K11" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="L11" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1070,7 +1297,7 @@
       <c r="C12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -1093,93 +1320,150 @@
       <c r="K12" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="L12" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+      <c r="A13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="4">
-        <f t="shared" si="0"/>
+      <c r="G13" s="13">
+        <f>LEN(F13)</f>
         <v>21</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="4">
-        <f t="shared" si="1"/>
+      <c r="I13" s="13">
+        <f>LEN(H13)</f>
         <v>22</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" ref="G14" si="2">LEN(F14)</f>
+        <v>2</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" ref="I14" si="3">LEN(H14)</f>
+        <v>2</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>56</v>
       </c>
       <c r="D16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="D17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="D18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
     </row>
@@ -1216,7 +1500,27 @@
     <hyperlink ref="K11" r:id="rId29" display="https://pub.e-tervis.ee/oids.py/viewform?oid=1.3.6.1.4.1.28284.6.2.1.156" xr:uid="{4CACA040-7D98-40CD-A2FE-092356F0121F}"/>
     <hyperlink ref="K12" r:id="rId30" display="https://pub.e-tervis.ee/oids.py/viewform?oid=1.3.6.1.4.1.28284.6.2.1.363" xr:uid="{8E4A8018-9B0A-4D2F-A829-B86DD5B89914}"/>
     <hyperlink ref="K13" r:id="rId31" display="https://pub.e-tervis.ee/oids.py/viewform?oid=1.3.6.1.4.1.28284.6.2.3.1" xr:uid="{B3E44F6B-7918-439F-8245-BD2408FF47A9}"/>
+    <hyperlink ref="N5" r:id="rId32" xr:uid="{49B89809-168D-7247-8C2B-A2E0C3980162}"/>
+    <hyperlink ref="N4" r:id="rId33" xr:uid="{8F99144D-F89F-1345-A94B-A4DCB1B2F8A1}"/>
+    <hyperlink ref="N3" r:id="rId34" xr:uid="{9D2ED72D-B520-4944-9F0E-20437C4ABB6F}"/>
+    <hyperlink ref="M5" r:id="rId35" xr:uid="{18595879-5BF1-974F-A630-18C010129AC2}"/>
+    <hyperlink ref="K14" r:id="rId36" display="https://pub.e-tervis.ee/oids.py/viewform?oid=1.3.6.1.4.1.28284.6.2.3.1" xr:uid="{1D0F9D8F-749C-0B4E-8EF3-D1E3F3B9B20C}"/>
+    <hyperlink ref="J14" r:id="rId37" xr:uid="{29EC62A3-FF67-8B41-B441-4E03B263D2B4}"/>
+    <hyperlink ref="B14" r:id="rId38" xr:uid="{DE2634B9-626F-7A40-B27D-7755BD903AA1}"/>
+    <hyperlink ref="N14" r:id="rId39" xr:uid="{734A26BB-A58B-8E43-96E4-46B2875E0998}"/>
+    <hyperlink ref="L7" r:id="rId40" xr:uid="{FA8728BD-773A-9C4B-AD53-9624349F750E}"/>
+    <hyperlink ref="N6" r:id="rId41" xr:uid="{3DF00ADC-75D0-BF41-91F5-1E0C3FAAF7BC}"/>
+    <hyperlink ref="N7" r:id="rId42" xr:uid="{9135B291-F3DB-D440-9F23-6BAC9B4A68C7}"/>
+    <hyperlink ref="N8" r:id="rId43" xr:uid="{901365AF-4AEA-8840-9ACB-7D5D5A1A44CF}"/>
+    <hyperlink ref="N9" r:id="rId44" xr:uid="{79AE07B5-C6FD-6B4B-846A-2BE95A64F028}"/>
+    <hyperlink ref="L9" r:id="rId45" xr:uid="{CF3289CF-E5BE-E648-812B-ACAC3FF2CF66}"/>
+    <hyperlink ref="L11" r:id="rId46" xr:uid="{901541C9-7C2D-144E-AF1C-367B4B857E26}"/>
+    <hyperlink ref="L2" r:id="rId47" xr:uid="{1FBE2E7E-6E47-9A45-8115-55DD1A2986EB}"/>
+    <hyperlink ref="N10" r:id="rId48" xr:uid="{C13A7BE2-0D4D-7944-91BF-990FCCC5D6EB}"/>
+    <hyperlink ref="N11" r:id="rId49" xr:uid="{6E5928C0-AC1B-7B46-AEC2-BB5F5F358128}"/>
+    <hyperlink ref="L12" r:id="rId50" xr:uid="{7FBA2CD8-9F1C-0946-AD63-AF49B3EBACBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId51"/>
 </worksheet>
 </file>
</xml_diff>